<commit_message>
Added average math and reading scores by grade.
</commit_message>
<xml_diff>
--- a/Resources/Weekly Schedule.xlsx
+++ b/Resources/Weekly Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carly/Desktop/Analysis Projects/School_District_Analysis/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FCC1F1-DEB3-DA48-812D-D51D8DEEF997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6CF006-9AB1-F040-921D-ECF111DDA697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="4" xr2:uid="{40C033E0-214D-4A92-9A34-B00EC3F0D799}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="4" xr2:uid="{40C033E0-214D-4A92-9A34-B00EC3F0D799}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Schedule" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Week 4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="118">
   <si>
     <t>Sunday</t>
   </si>
@@ -383,6 +382,15 @@
   </si>
   <si>
     <t>2:00 pm - 2:30 pm</t>
+  </si>
+  <si>
+    <t>Lesson 4.8</t>
+  </si>
+  <si>
+    <t>Lesson 4.9</t>
+  </si>
+  <si>
+    <t>Worked out</t>
   </si>
 </sst>
 </file>
@@ -2417,7 +2425,7 @@
   <dimension ref="B1:I33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2507,6 +2515,9 @@
       <c r="G6">
         <v>2.25</v>
       </c>
+      <c r="I6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
@@ -2557,33 +2568,106 @@
       <c r="D11" t="s">
         <v>109</v>
       </c>
+      <c r="E11" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="F11" s="25" t="s">
         <v>114</v>
       </c>
       <c r="G11">
         <v>0.5</v>
       </c>
+      <c r="I11" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="18">
+        <v>44650</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="18">
+        <v>44651</v>
+      </c>
+      <c r="D16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C17" s="18"/>
+      <c r="D17" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="E17" s="26"/>
+      <c r="F17" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="7:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="18">
+        <v>44652</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F20" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G32" s="31">
         <f>SUM(G2:G31)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added scores by school type.
</commit_message>
<xml_diff>
--- a/Resources/Weekly Schedule.xlsx
+++ b/Resources/Weekly Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carly/Desktop/Analysis Projects/School_District_Analysis/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6CF006-9AB1-F040-921D-ECF111DDA697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C59339B-9E95-4340-AE58-FC5C22A9969D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="4" xr2:uid="{40C033E0-214D-4A92-9A34-B00EC3F0D799}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="4" xr2:uid="{40C033E0-214D-4A92-9A34-B00EC3F0D799}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Schedule" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="127">
   <si>
     <t>Sunday</t>
   </si>
@@ -391,6 +391,33 @@
   </si>
   <si>
     <t>Worked out</t>
+  </si>
+  <si>
+    <t>Break | Will's Birthday</t>
+  </si>
+  <si>
+    <t>Lesson 4.10</t>
+  </si>
+  <si>
+    <t>11:30 am -  12:10 pm</t>
+  </si>
+  <si>
+    <t>Lesson 4.11</t>
+  </si>
+  <si>
+    <t>12:10 pm - 12:45 pm</t>
+  </si>
+  <si>
+    <t>Lesson 4.12</t>
+  </si>
+  <si>
+    <t>12:45 pm - 1:00 pm</t>
+  </si>
+  <si>
+    <t>Lesson 4.13</t>
+  </si>
+  <si>
+    <t>1:00 pm - 1:30 pm</t>
   </si>
 </sst>
 </file>
@@ -2422,252 +2449,312 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90BB1E0-FCC4-D14B-857F-2CA6202E576B}">
-  <dimension ref="B1:I33"/>
+  <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G1" s="27" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="18">
         <v>44647</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.75</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F5" s="32"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G5" s="32"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="18">
         <v>44648</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2.25</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D7" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
         <v>107</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="25" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="18">
         <v>44649</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
         <v>113</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.5</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.5</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="18">
         <v>44650</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>2</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="18">
         <v>44651</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="18"/>
+      <c r="E16" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C17" s="18"/>
-      <c r="D17" t="s">
+      <c r="D17" s="18"/>
+      <c r="E17" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F18" s="26"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="18">
         <v>44652</v>
       </c>
-      <c r="F19" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F20" s="25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G32" s="31">
-        <f>SUM(G2:G31)</f>
-        <v>14</v>
+      <c r="D19" s="18"/>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" s="26"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="18">
+        <v>44653</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="31">
+        <f>SUM(H2:H31)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="33" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>

</xml_diff>